<commit_message>
Update .mxproject, subdir.mk, and 1078 more files...
</commit_message>
<xml_diff>
--- a/pcb/BOM_stm32audio_board_v2_parts.xlsx
+++ b/pcb/BOM_stm32audio_board_v2_parts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aron\Documents\GitHub\Digital_guitar_effect\pcb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\git\onlab\Digital_guitar_effect\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A3021E-0894-4AEB-83DC-A016D3795821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2C8B6D-7A2E-4D73-BE7B-DFC5CAD20A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{C1ECC89A-70EF-4060-9F61-ECE5038C6326}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="34560" windowHeight="18600" xr2:uid="{C1ECC89A-70EF-4060-9F61-ECE5038C6326}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Type</t>
   </si>
@@ -87,6 +85,18 @@
   </si>
   <si>
     <t>https://hu.farnell.com/microchip/mic2920a-3-3ws-tr/ldo-reg-26vin-0-4a-3-3v-3sot223/dp/2510013?ICID=I-RP-STM7REC-0</t>
+  </si>
+  <si>
+    <t>18 to 5 V DCDC</t>
+  </si>
+  <si>
+    <t>https://hu.farnell.com/diodes-inc/ap1509-50sg-13/ic-buck-reg-5v-2a-8sop/dp/1825323</t>
+  </si>
+  <si>
+    <t>DIODES INC. AP1509-50SG-13</t>
+  </si>
+  <si>
+    <t>SOP-8L</t>
   </si>
 </sst>
 </file>
@@ -476,16 +486,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFBBC6E-FF7A-4C12-8012-F4C4CA447A76}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="82.44140625" customWidth="1"/>
     <col min="5" max="5" width="22.21875" customWidth="1"/>
@@ -557,6 +567,20 @@
       </c>
       <c r="E4">
         <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Capacitor types are choosen, schematic updated, unused capacitors deleted. Connectors need to be connected to the mcu and its finished
</commit_message>
<xml_diff>
--- a/pcb/BOM_stm32audio_board_v2_parts.xlsx
+++ b/pcb/BOM_stm32audio_board_v2_parts.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\git\onlab\Digital_guitar_effect\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2C8B6D-7A2E-4D73-BE7B-DFC5CAD20A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C11CF35-F1B3-4D48-AD36-0DA8DE8764FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="34560" windowHeight="18600" xr2:uid="{C1ECC89A-70EF-4060-9F61-ECE5038C6326}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" activeTab="1" xr2:uid="{C1ECC89A-70EF-4060-9F61-ECE5038C6326}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="capacitors" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Type</t>
   </si>
@@ -97,6 +98,27 @@
   </si>
   <si>
     <t>SOP-8L</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>https://www.hestore.hu/prod_10024356.html</t>
+  </si>
+  <si>
+    <t>100nf</t>
+  </si>
+  <si>
+    <t>50V</t>
   </si>
 </sst>
 </file>
@@ -488,7 +510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFBBC6E-FF7A-4C12-8012-F4C4CA447A76}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
@@ -590,4 +612,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9A4E0F3-2EE4-4A98-905A-4A2F0718964D}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2">
+        <v>603</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
pcb seems to be finished drc error: 0
</commit_message>
<xml_diff>
--- a/pcb/BOM_stm32audio_board_v2_parts.xlsx
+++ b/pcb/BOM_stm32audio_board_v2_parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\git\onlab\Digital_guitar_effect\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402DAF10-C050-41F6-960D-0A25C8927CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A50568-E35E-49FA-ABC3-97A9052B7916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" activeTab="1" xr2:uid="{C1ECC89A-70EF-4060-9F61-ECE5038C6326}"/>
+    <workbookView xWindow="-23016" yWindow="216" windowWidth="23016" windowHeight="12216" xr2:uid="{C1ECC89A-70EF-4060-9F61-ECE5038C6326}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -510,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFBBC6E-FF7A-4C12-8012-F4C4CA447A76}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,16 +601,17 @@
       <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{3266427D-D256-43AA-8CC4-40F136652AAD}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{0A22B357-1643-4D24-889B-13E9BEB73C64}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -618,7 +619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9A4E0F3-2EE4-4A98-905A-4A2F0718964D}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>

</xml_diff>